<commit_message>
agaramudhali - initial - full working version
</commit_message>
<xml_diff>
--- a/analysis/thirukkural-agara-mudhali/first-character-data.xlsx
+++ b/analysis/thirukkural-agara-mudhali/first-character-data.xlsx
@@ -2,38 +2,41 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\spring-boot-learning\data-jpa-sqlite\analysis\thirukkural-agara-mudhali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E69735-6426-4FE2-A5FA-10D9B2D81332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F39A763-19CB-406E-B702-7A0DD39191FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Squirrel SQL Export" sheetId="1" r:id="rId1"/>
     <sheet name="line1-first-letter" sheetId="2" r:id="rId2"/>
-    <sheet name="line1-unique-first-letter" sheetId="3" r:id="rId3"/>
-    <sheet name="letter-totalcount" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
-    <sheet name="unique-letters" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
+    <sheet name="line1-unique-first-letter" sheetId="3" r:id="rId4"/>
+    <sheet name="letter-totalcount" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId6"/>
+    <sheet name="unique-letters" sheetId="6" r:id="rId7"/>
+    <sheet name="count-grouped" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'line1-first-letter'!$A$1:$A$1081</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Squirrel SQL Export'!$A$1:$B$1081</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'unique-letters'!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="5" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2479" uniqueCount="1317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2577" uniqueCount="1318">
   <si>
     <t>line1_without_punctuation</t>
   </si>
@@ -3984,13 +3987,16 @@
   </si>
   <si>
     <t>Character Byte Length</t>
+  </si>
+  <si>
+    <t>letter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -4001,6 +4007,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4053,7 +4067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8810,7 +8824,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4BD692F5-7525-488D-A70A-9A86004429CB}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4BD692F5-7525-488D-A70A-9A86004429CB}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E3:F75" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -9131,7 +9145,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{77D50400-A635-4D8D-90E3-DD18B1183C0F}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Character Byte Length">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{77D50400-A635-4D8D-90E3-DD18B1183C0F}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Character Byte Length">
   <location ref="G2:H5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0"/>
@@ -19260,23 +19274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE66164B-ABE0-475B-8097-FA7CE393B951}">
   <dimension ref="A1:F1081"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68:F74"/>
-      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" axis="axisRow" start="64" max="72" activeRow="67" activeCol="4" previousRow="73" previousCol="4" click="1" r:id="rId1">
-        <pivotArea dataOnly="0" axis="axisRow" fieldPosition="0">
-          <references count="1">
-            <reference field="0" count="7">
-              <x v="64"/>
-              <x v="65"/>
-              <x v="66"/>
-              <x v="67"/>
-              <x v="68"/>
-              <x v="69"/>
-              <x v="70"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotSelection>
+    <sheetView topLeftCell="A64" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -33788,10 +33787,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD72218-8531-4415-8296-44393AF97611}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE86253-F4BA-4F37-89A9-5BB151C9DD41}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -33837,7 +33848,7 @@
       <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3">
         <v>18</v>
       </c>
     </row>
@@ -33852,7 +33863,7 @@
       <c r="G4" s="4">
         <v>2</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4">
         <v>53</v>
       </c>
     </row>
@@ -33867,7 +33878,7 @@
       <c r="G5" s="4" t="s">
         <v>1307</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5">
         <v>71</v>
       </c>
     </row>
@@ -34482,12 +34493,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6154262A-673D-443D-96F1-065A6E31C75E}">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -35081,12 +35092,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C388502-3B6E-475F-B606-5DE0C1761C84}">
   <dimension ref="A2:B72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B72"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -35738,117 +35749,937 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7347AF29-A3E0-40C0-854E-1FAC744760DE}">
-  <dimension ref="A2:A21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="5" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>1287</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>1313</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
         <v>1288</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>1289</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+      <c r="B9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
         <v>1291</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>1292</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>1293</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>1294</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>1296</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>1297</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>1298</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>1304</v>
+      </c>
+      <c r="B13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B14">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
         <v>1299</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>1300</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>1301</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B18">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
         <v>1302</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B20">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B21">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B21">
+    <sortCondition ref="B2:B21"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21697553-47DD-42F3-AAEE-B41DB765B367}">
+  <dimension ref="B1:K74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="9.9453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.68359375" customWidth="1"/>
+    <col min="11" max="11" width="12.47265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="J1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1309</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="K2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C3">
+        <v>141</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="K3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C4">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1289</v>
+      </c>
+      <c r="K4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C5">
+        <v>102</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1290</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1291</v>
+      </c>
+      <c r="K6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C7">
+        <v>60</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1292</v>
+      </c>
+      <c r="K7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1293</v>
+      </c>
+      <c r="K8">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C9">
+        <v>41</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1294</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1295</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1296</v>
+      </c>
+      <c r="K11">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C12">
+        <v>37</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1297</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1298</v>
+      </c>
+      <c r="K13">
+        <f>SUM(C14:C22)</f>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C14">
+        <v>54</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1299</v>
+      </c>
+      <c r="K14">
+        <f>SUM(C23:C30)</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1313</v>
+      </c>
+      <c r="K15">
+        <f>SUM(C31:C31)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C16">
+        <v>27</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1300</v>
+      </c>
+      <c r="K16">
+        <f>SUM(C32:C41)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1301</v>
+      </c>
+      <c r="K17">
+        <f>SUM(C42:C49)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1302</v>
+      </c>
+      <c r="K18">
+        <f>SUM(C50:C58)</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="J19" t="s">
         <v>1303</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
+      <c r="K19">
+        <f>SUM(C59:C65)</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="J20" t="s">
         <v>1314</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
+      <c r="K20">
+        <f>SUM(C66:C66)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C21">
+        <v>15</v>
+      </c>
+      <c r="J21" t="s">
         <v>1304</v>
+      </c>
+      <c r="K21">
+        <f>SUM(C67:C73)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <f>SUM(K2:K21)</f>
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C29">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C32">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C36">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C42">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C44">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C50">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C52">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C54">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C55">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C56">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C57">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B59" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C59">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B60" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B61" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B62" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C62">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B63" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B64" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B65" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B66" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C66">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B67" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C67">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B68" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C68">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B69" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C69">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B70" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B71" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B72" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C72">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B73" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B74" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C74">
+        <v>1080</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>